<commit_message>
Ultimas pruebas de tiempos y esfuerzos. Cambios al codigo para asegurar funcionamiento correcto en revisión y defensa final. Memoria acabada [No subida]
</commit_message>
<xml_diff>
--- a/measures/elapsed_times_automatization.xlsx
+++ b/measures/elapsed_times_automatization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\MASTER\S2\TM_Distribuidos\Repository\measures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE33FB58-8C08-45F7-ABFB-2C4967FB6CE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE2B549-F96C-4C2B-92D9-8CE1A5E47B22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{616A3160-F3AC-4E7C-8D36-813A6B21A352}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t># Threads (One user per thread)</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>10,02 s.</t>
+  </si>
+  <si>
+    <t>(1 per sec.)</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Tiempo de recepción en misma sala:</t>
+  </si>
+  <si>
+    <t>#Msg</t>
+  </si>
+  <si>
+    <t>1.42</t>
   </si>
 </sst>
 </file>
@@ -150,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,6 +176,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C63B54-F57C-44AA-9179-0A957EBC77C8}">
-  <dimension ref="B1:D67"/>
+  <dimension ref="B1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,26 +505,31 @@
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,12 +538,25 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>50</v>
       </c>
@@ -525,8 +564,25 @@
         <v>4</v>
       </c>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>60</v>
       </c>
@@ -534,8 +590,25 @@
         <v>27</v>
       </c>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1">
+        <v>50</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>70</v>
       </c>
@@ -543,8 +616,25 @@
         <v>3</v>
       </c>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1">
+        <v>50</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>80</v>
       </c>
@@ -552,8 +642,25 @@
         <v>5</v>
       </c>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>30</v>
+      </c>
+      <c r="I10" s="1">
+        <v>50</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2.79</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>90</v>
       </c>
@@ -561,8 +668,25 @@
         <v>6</v>
       </c>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>50</v>
+      </c>
+      <c r="I11" s="1">
+        <v>50</v>
+      </c>
+      <c r="J11" s="1">
+        <v>5.13</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>100</v>
       </c>
@@ -570,8 +694,25 @@
         <v>8</v>
       </c>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>100</v>
+      </c>
+      <c r="I12" s="1">
+        <v>50</v>
+      </c>
+      <c r="J12" s="1">
+        <v>14.22</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>200</v>
       </c>
@@ -579,8 +720,25 @@
         <v>7</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1">
+        <v>150</v>
+      </c>
+      <c r="I13" s="1">
+        <v>50</v>
+      </c>
+      <c r="J13" s="1">
+        <v>28.02</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>400</v>
       </c>
@@ -588,8 +746,25 @@
         <v>9</v>
       </c>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1">
+        <v>200</v>
+      </c>
+      <c r="I14" s="1">
+        <v>50</v>
+      </c>
+      <c r="J14" s="1">
+        <v>52.03</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1000</v>
       </c>
@@ -597,8 +772,25 @@
         <v>10</v>
       </c>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1">
+        <v>250</v>
+      </c>
+      <c r="I15" s="1">
+        <v>50</v>
+      </c>
+      <c r="J15" s="1">
+        <v>89.63</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>2000</v>
       </c>
@@ -606,8 +798,19 @@
         <v>11</v>
       </c>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>5000</v>
       </c>
@@ -615,8 +818,19 @@
         <v>15</v>
       </c>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>10000</v>
       </c>
@@ -624,8 +838,19 @@
         <v>16</v>
       </c>
       <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>20000</v>
       </c>
@@ -633,8 +858,19 @@
         <v>17</v>
       </c>
       <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>30000</v>
       </c>
@@ -642,8 +878,19 @@
         <v>19</v>
       </c>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>40000</v>
       </c>
@@ -651,8 +898,19 @@
         <v>20</v>
       </c>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>50000</v>
       </c>
@@ -660,50 +918,149 @@
         <v>18</v>
       </c>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>14</v>
       </c>
@@ -711,13 +1068,35 @@
         <v>1</v>
       </c>
       <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>10</v>
       </c>
@@ -725,8 +1104,19 @@
         <v>26</v>
       </c>
       <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>25</v>
       </c>
@@ -734,8 +1124,19 @@
         <v>24</v>
       </c>
       <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>50</v>
       </c>
@@ -743,8 +1144,19 @@
         <v>25</v>
       </c>
       <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>100</v>
       </c>
@@ -752,8 +1164,19 @@
         <v>21</v>
       </c>
       <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>200</v>
       </c>
@@ -761,8 +1184,19 @@
         <v>22</v>
       </c>
       <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>300</v>
       </c>
@@ -770,8 +1204,19 @@
         <v>23</v>
       </c>
       <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>400</v>
       </c>
@@ -779,48 +1224,70 @@
         <v>24</v>
       </c>
       <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -921,9 +1388,10 @@
       <c r="D67" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B29:C29"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>